<commit_message>
Build Clean Data Tables
</commit_message>
<xml_diff>
--- a/Volume by Region Data Request v3.xlsx
+++ b/Volume by Region Data Request v3.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahil\Documents\Github\excelprogress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DC5D69E-6B45-4131-BE5A-7D276679369E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FDCEB7-A125-43CB-8350-86162D56AF41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" tabRatio="458" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" tabRatio="458" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Email" sheetId="73" r:id="rId1"/>
     <sheet name="EXT0070122021 OG" sheetId="75" state="hidden" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="77" r:id="rId3"/>
+    <sheet name="Summary" sheetId="78" r:id="rId3"/>
     <sheet name="Pivot" sheetId="76" r:id="rId4"/>
     <sheet name="Volume Data" sheetId="72" r:id="rId5"/>
     <sheet name="Sheet3 OG" sheetId="74" state="hidden" r:id="rId6"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3375" uniqueCount="950">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3263" uniqueCount="961">
   <si>
     <t>CLID</t>
   </si>
@@ -2918,18 +2918,52 @@
   </si>
   <si>
     <t xml:space="preserve">same store sales slower than expected in Q2 vs Q1 in YOY, comprising of majority of remaining variance </t>
+  </si>
+  <si>
+    <t>- NAM client onboarding in Q2 2020 anniversaried in Q2 2021, slowing perceived growth</t>
+  </si>
+  <si>
+    <t>Q2 2021 Overview</t>
+  </si>
+  <si>
+    <t>All data as of 2/10/2022</t>
+  </si>
+  <si>
+    <t>Number of Customers YOY</t>
+  </si>
+  <si>
+    <t>Volume YOY</t>
+  </si>
+  <si>
+    <t>Distribution by Region</t>
+  </si>
+  <si>
+    <t>Data With Variance</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>Prior Year</t>
+  </si>
+  <si>
+    <t>% Change</t>
+  </si>
+  <si>
+    <t>H1 YoY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
+    <numFmt numFmtId="166" formatCode="0,&quot;k&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="ARIAL"/>
@@ -2956,13 +2990,70 @@
       <name val="ARIAL"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="10"/>
+      <name val="ARIAL"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="ARIAL"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <name val="ARIAL"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="24"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -2991,7 +3082,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -3042,6 +3133,61 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="2" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -3049,7 +3195,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Text UPPER lower" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
-  <dxfs count="67">
+  <dxfs count="66">
     <dxf>
       <font>
         <b val="0"/>
@@ -3280,9 +3426,6 @@
     </dxf>
     <dxf>
       <alignment wrapText="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -15683,23 +15826,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{8B428AE4-E774-4CE8-97EC-404D39F1F4CC}" name="Table5" displayName="Table5" ref="A1:H29" totalsRowShown="0">
-  <autoFilter ref="A1:H29" xr:uid="{8B428AE4-E774-4CE8-97EC-404D39F1F4CC}"/>
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{1CDCD11C-7559-4D60-926A-FEA8FCEA1711}" name="CLID"/>
-    <tableColumn id="2" xr3:uid="{1FB599A4-0D12-43C4-95E3-48CBC7B8F1B9}" name="Date" dataDxfId="66"/>
-    <tableColumn id="3" xr3:uid="{BBF891A3-B9BB-4CB2-AB23-59B0152575E2}" name="Vol"/>
-    <tableColumn id="4" xr3:uid="{89AEAA78-E28E-45BE-BCCA-49E576CC1B74}" name="LEN"/>
-    <tableColumn id="5" xr3:uid="{9B6D4E26-0525-4A95-9621-2E256C9C3D2C}" name="Index Math Region ID"/>
-    <tableColumn id="6" xr3:uid="{F8CB2830-AC13-49FF-9830-4E20AFB79C73}" name="Region Name"/>
-    <tableColumn id="7" xr3:uid="{10307EC2-C0FA-4652-B17F-342200520760}" name="Quarter"/>
-    <tableColumn id="8" xr3:uid="{FFCCD3DA-3B82-4EF7-B02F-C4A64DCC9AC3}" name="Quarter by Vlookup"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{406B180F-939D-4E8E-A198-0941B7059A16}" name="VolumebyClient" displayName="VolumebyClient" ref="A1:H908" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A1:H908" xr:uid="{406B180F-939D-4E8E-A198-0941B7059A16}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H908">
@@ -15729,7 +15855,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{14F98703-7709-4799-96B7-DEF2AB592176}" name="Quarters" displayName="Quarters" ref="P1:R7" totalsRowShown="0" headerRowDxfId="20">
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0CBD38A7-5922-499C-B3C6-C1D4D12C14A8}" name="Date Start" dataDxfId="19">
@@ -15742,7 +15868,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E311F35B-2E55-4952-8583-E766E50A2002}" name="GeobyClient" displayName="GeobyClient" ref="A1:G54" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:G54" xr:uid="{E311F35B-2E55-4952-8583-E766E50A2002}"/>
   <tableColumns count="7">
@@ -15768,7 +15894,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{73CE4639-4172-46C1-8556-28321ADFD967}" name="GEONames" displayName="GEONames" ref="J1:L6" totalsRowCount="1" headerRowDxfId="7" dataDxfId="6">
   <autoFilter ref="J1:L5" xr:uid="{73CE4639-4172-46C1-8556-28321ADFD967}"/>
   <tableColumns count="3">
@@ -16105,7 +16231,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5EF340-377D-43B0-A32D-A2F3BF14766B}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="J52" sqref="J52"/>
     </sheetView>
   </sheetViews>
@@ -24566,780 +24692,484 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4076FFD-9089-40D8-A4F8-7A01C3F13154}">
-  <dimension ref="A1:H29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F675FF-8571-44E8-8591-11391A021DF3}">
+  <dimension ref="B1:N41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H29"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4" style="3" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="3"/>
+    <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" style="3"/>
+    <col min="9" max="9" width="4.42578125" style="3" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="3"/>
+    <col min="12" max="12" width="4.42578125" style="3" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="2:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B1" s="25" t="s">
+        <v>951</v>
+      </c>
+    </row>
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="24" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>947</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="7" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B10" s="26" t="s">
+        <v>953</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B11" s="26" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B13" s="26" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="15" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B15" s="26" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="20.25" x14ac:dyDescent="0.2">
+      <c r="B18" s="32" t="s">
+        <v>906</v>
+      </c>
+      <c r="C18" s="27"/>
+      <c r="F18" s="32" t="s">
+        <v>957</v>
+      </c>
+      <c r="G18" s="27"/>
+    </row>
+    <row r="19" spans="2:7" ht="30" x14ac:dyDescent="0.2">
+      <c r="B19" s="34">
+        <f>Pivot!G40</f>
+        <v>965282</v>
+      </c>
+      <c r="C19" s="33"/>
+      <c r="F19" s="33">
+        <f>Pivot!$I$121</f>
+        <v>50</v>
+      </c>
+      <c r="G19" s="33"/>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="29" t="s">
+        <v>958</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>959</v>
+      </c>
+      <c r="F20" s="29" t="s">
+        <v>958</v>
+      </c>
+      <c r="G20" s="28" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="35">
+        <f>Pivot!C40</f>
+        <v>940140</v>
+      </c>
+      <c r="C21" s="37">
+        <f>B19/B21-1</f>
+        <v>2.6742825536622217E-2</v>
+      </c>
+      <c r="F21" s="31">
+        <f>SUM(F17:F19)</f>
+        <v>50</v>
+      </c>
+      <c r="G21" s="30">
+        <f>F19/F21-1</f>
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" t="s">
-        <v>901</v>
-      </c>
-      <c r="E1" t="s">
-        <v>905</v>
-      </c>
-      <c r="F1" t="s">
-        <v>909</v>
-      </c>
-      <c r="G1" t="s">
-        <v>910</v>
-      </c>
-      <c r="H1" t="s">
-        <v>920</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43921</v>
-      </c>
-      <c r="C2">
-        <v>884</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
-      </c>
-      <c r="E2" t="s">
-        <v>55</v>
-      </c>
-      <c r="F2" t="s">
+    </row>
+    <row r="35" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+      <c r="B35" s="38" t="s">
+        <v>906</v>
+      </c>
+      <c r="C35" s="39"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="39"/>
+      <c r="H35" s="39"/>
+      <c r="J35" s="40" t="s">
+        <v>935</v>
+      </c>
+      <c r="K35" s="41"/>
+      <c r="M35" s="40" t="s">
+        <v>960</v>
+      </c>
+      <c r="N35" s="41"/>
+    </row>
+    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B36" s="42" t="s">
+        <v>921</v>
+      </c>
+      <c r="C36" s="43" t="s">
+        <v>914</v>
+      </c>
+      <c r="D36" s="43" t="s">
+        <v>915</v>
+      </c>
+      <c r="E36" s="43" t="s">
+        <v>916</v>
+      </c>
+      <c r="F36" s="43" t="s">
+        <v>917</v>
+      </c>
+      <c r="G36" s="43" t="s">
+        <v>918</v>
+      </c>
+      <c r="H36" s="43" t="s">
+        <v>919</v>
+      </c>
+      <c r="J36" s="44" t="s">
+        <v>933</v>
+      </c>
+      <c r="K36" s="44" t="s">
+        <v>934</v>
+      </c>
+      <c r="M36" s="44" t="s">
+        <v>933</v>
+      </c>
+      <c r="N36" s="44" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B37" s="20" t="s">
+        <v>898</v>
+      </c>
+      <c r="C37" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B37,VolumebyClient[Quarter],Summary!C$36)</f>
+        <v>509419</v>
+      </c>
+      <c r="D37" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B37,VolumebyClient[Quarter],Summary!D$36)</f>
+        <v>576618</v>
+      </c>
+      <c r="E37" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B37,VolumebyClient[Quarter],Summary!E$36)</f>
+        <v>363694</v>
+      </c>
+      <c r="F37" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B37,VolumebyClient[Quarter],Summary!F$36)</f>
+        <v>432034</v>
+      </c>
+      <c r="G37" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B37,VolumebyClient[Quarter],Summary!G$36)</f>
+        <v>530019</v>
+      </c>
+      <c r="H37" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B37,VolumebyClient[Quarter],Summary!H$36)</f>
+        <v>596502</v>
+      </c>
+      <c r="J37" s="9">
+        <f>H37-D37</f>
+        <v>19884</v>
+      </c>
+      <c r="K37" s="45">
+        <f>H37/D37-1</f>
+        <v>3.4483835051975387E-2</v>
+      </c>
+      <c r="M37" s="9">
+        <f>SUM(G37:H37)-SUM(C37:D37)</f>
+        <v>40484</v>
+      </c>
+      <c r="N37" s="45">
+        <f>SUM(G37:H37)/SUM(C37:D37)-1</f>
+        <v>3.7276814694158666E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B38" s="20" t="s">
+        <v>899</v>
+      </c>
+      <c r="C38" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B38,VolumebyClient[Quarter],Summary!C$36)</f>
+        <v>147852</v>
+      </c>
+      <c r="D38" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B38,VolumebyClient[Quarter],Summary!D$36)</f>
+        <v>173566</v>
+      </c>
+      <c r="E38" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B38,VolumebyClient[Quarter],Summary!E$36)</f>
+        <v>103536</v>
+      </c>
+      <c r="F38" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B38,VolumebyClient[Quarter],Summary!F$36)</f>
+        <v>129264</v>
+      </c>
+      <c r="G38" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B38,VolumebyClient[Quarter],Summary!G$36)</f>
+        <v>150204</v>
+      </c>
+      <c r="H38" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B38,VolumebyClient[Quarter],Summary!H$36)</f>
+        <v>176338</v>
+      </c>
+      <c r="J38" s="9">
+        <f t="shared" ref="J38:J41" si="0">H38-D38</f>
+        <v>2772</v>
+      </c>
+      <c r="K38" s="45">
+        <f t="shared" ref="K38:K41" si="1">H38/D38-1</f>
+        <v>1.5970869870827187E-2</v>
+      </c>
+      <c r="M38" s="9">
+        <f t="shared" ref="M38:M41" si="2">SUM(G38:H38)-SUM(C38:D38)</f>
+        <v>5124</v>
+      </c>
+      <c r="N38" s="45">
+        <f t="shared" ref="N38:N41" si="3">SUM(G38:H38)/SUM(C38:D38)-1</f>
+        <v>1.5941857643318125E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B39" s="20" t="s">
+        <v>908</v>
+      </c>
+      <c r="C39" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B39,VolumebyClient[Quarter],Summary!C$36)</f>
+        <v>95736</v>
+      </c>
+      <c r="D39" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B39,VolumebyClient[Quarter],Summary!D$36)</f>
+        <v>107338</v>
+      </c>
+      <c r="E39" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B39,VolumebyClient[Quarter],Summary!E$36)</f>
+        <v>69198</v>
+      </c>
+      <c r="F39" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B39,VolumebyClient[Quarter],Summary!F$36)</f>
+        <v>80144</v>
+      </c>
+      <c r="G39" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B39,VolumebyClient[Quarter],Summary!G$36)</f>
+        <v>99778</v>
+      </c>
+      <c r="H39" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B39,VolumebyClient[Quarter],Summary!H$36)</f>
+        <v>109811</v>
+      </c>
+      <c r="J39" s="9">
+        <f t="shared" si="0"/>
+        <v>2473</v>
+      </c>
+      <c r="K39" s="45">
+        <f t="shared" si="1"/>
+        <v>2.3039370959026639E-2</v>
+      </c>
+      <c r="M39" s="9">
+        <f t="shared" si="2"/>
+        <v>6515</v>
+      </c>
+      <c r="N39" s="45">
+        <f t="shared" si="3"/>
+        <v>3.2081901178880656E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B40" s="20" t="s">
         <v>907</v>
       </c>
-      <c r="G2" t="s">
-        <v>914</v>
-      </c>
-      <c r="H2" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="1">
-        <v>43921</v>
-      </c>
-      <c r="C3">
-        <v>4248</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" t="s">
-        <v>907</v>
-      </c>
-      <c r="G3" t="s">
-        <v>914</v>
-      </c>
-      <c r="H3" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="1">
-        <v>43890</v>
-      </c>
-      <c r="C4">
-        <v>3827</v>
-      </c>
-      <c r="D4">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" t="s">
-        <v>907</v>
-      </c>
-      <c r="G4" t="s">
-        <v>914</v>
-      </c>
-      <c r="H4" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5" s="1">
-        <v>43861</v>
-      </c>
-      <c r="C5">
-        <v>3405</v>
-      </c>
-      <c r="D5">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" t="s">
-        <v>907</v>
-      </c>
-      <c r="G5" t="s">
-        <v>914</v>
-      </c>
-      <c r="H5" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" s="1">
-        <v>43921</v>
-      </c>
-      <c r="C6">
-        <v>1507</v>
-      </c>
-      <c r="D6">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" t="s">
-        <v>907</v>
-      </c>
-      <c r="G6" t="s">
-        <v>914</v>
-      </c>
-      <c r="H6" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="1">
-        <v>43890</v>
-      </c>
-      <c r="C7">
-        <v>1358</v>
-      </c>
-      <c r="D7">
-        <v>7</v>
-      </c>
-      <c r="E7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" t="s">
-        <v>907</v>
-      </c>
-      <c r="G7" t="s">
-        <v>914</v>
-      </c>
-      <c r="H7" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="1">
-        <v>43861</v>
-      </c>
-      <c r="C8">
-        <v>1211</v>
-      </c>
-      <c r="D8">
-        <v>7</v>
-      </c>
-      <c r="E8" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" t="s">
-        <v>907</v>
-      </c>
-      <c r="G8" t="s">
-        <v>914</v>
-      </c>
-      <c r="H8" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1">
-        <v>43921</v>
-      </c>
-      <c r="C9">
-        <v>375</v>
-      </c>
-      <c r="D9">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" t="s">
-        <v>907</v>
-      </c>
-      <c r="G9" t="s">
-        <v>914</v>
-      </c>
-      <c r="H9" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1">
-        <v>43890</v>
-      </c>
-      <c r="C10">
-        <v>304</v>
-      </c>
-      <c r="D10">
-        <v>7</v>
-      </c>
-      <c r="E10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F10" t="s">
-        <v>907</v>
-      </c>
-      <c r="G10" t="s">
-        <v>914</v>
-      </c>
-      <c r="H10" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="1">
-        <v>43861</v>
-      </c>
-      <c r="C11">
-        <v>303</v>
-      </c>
-      <c r="D11">
-        <v>7</v>
-      </c>
-      <c r="E11" t="s">
-        <v>55</v>
-      </c>
-      <c r="F11" t="s">
-        <v>907</v>
-      </c>
-      <c r="G11" t="s">
-        <v>914</v>
-      </c>
-      <c r="H11" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="1">
-        <v>43861</v>
-      </c>
-      <c r="C12">
-        <v>756</v>
-      </c>
-      <c r="D12">
-        <v>7</v>
-      </c>
-      <c r="E12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F12" t="s">
-        <v>907</v>
-      </c>
-      <c r="G12" t="s">
-        <v>914</v>
-      </c>
-      <c r="H12" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="1">
-        <v>43890</v>
-      </c>
-      <c r="C13">
-        <v>954</v>
-      </c>
-      <c r="D13">
-        <v>7</v>
-      </c>
-      <c r="E13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" t="s">
-        <v>907</v>
-      </c>
-      <c r="G13" t="s">
-        <v>914</v>
-      </c>
-      <c r="H13" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="1">
-        <v>43921</v>
-      </c>
-      <c r="C14">
-        <v>955</v>
-      </c>
-      <c r="D14">
-        <v>7</v>
-      </c>
-      <c r="E14" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" t="s">
-        <v>907</v>
-      </c>
-      <c r="G14" t="s">
-        <v>914</v>
-      </c>
-      <c r="H14" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" s="1">
-        <v>43921</v>
-      </c>
-      <c r="C15">
-        <v>609</v>
-      </c>
-      <c r="D15">
-        <v>7</v>
-      </c>
-      <c r="E15" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" t="s">
-        <v>907</v>
-      </c>
-      <c r="G15" t="s">
-        <v>914</v>
-      </c>
-      <c r="H15" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="1">
-        <v>43890</v>
-      </c>
-      <c r="C16">
-        <v>546</v>
-      </c>
-      <c r="D16">
-        <v>7</v>
-      </c>
-      <c r="E16" t="s">
-        <v>55</v>
-      </c>
-      <c r="F16" t="s">
-        <v>907</v>
-      </c>
-      <c r="G16" t="s">
-        <v>914</v>
-      </c>
-      <c r="H16" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>43861</v>
-      </c>
-      <c r="C17">
-        <v>484</v>
-      </c>
-      <c r="D17">
-        <v>7</v>
-      </c>
-      <c r="E17" t="s">
-        <v>55</v>
-      </c>
-      <c r="F17" t="s">
-        <v>907</v>
-      </c>
-      <c r="G17" t="s">
-        <v>914</v>
-      </c>
-      <c r="H17" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="1">
-        <v>43861</v>
-      </c>
-      <c r="C18">
-        <v>188</v>
-      </c>
-      <c r="D18">
-        <v>7</v>
-      </c>
-      <c r="E18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" t="s">
-        <v>907</v>
-      </c>
-      <c r="G18" t="s">
-        <v>914</v>
-      </c>
-      <c r="H18" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1">
-        <v>43890</v>
-      </c>
-      <c r="C19">
-        <v>168</v>
-      </c>
-      <c r="D19">
-        <v>7</v>
-      </c>
-      <c r="E19" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" t="s">
-        <v>907</v>
-      </c>
-      <c r="G19" t="s">
-        <v>914</v>
-      </c>
-      <c r="H19" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="1">
-        <v>43921</v>
-      </c>
-      <c r="C20">
-        <v>226</v>
-      </c>
-      <c r="D20">
-        <v>7</v>
-      </c>
-      <c r="E20" t="s">
-        <v>55</v>
-      </c>
-      <c r="F20" t="s">
-        <v>907</v>
-      </c>
-      <c r="G20" t="s">
-        <v>914</v>
-      </c>
-      <c r="H20" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="1">
-        <v>43921</v>
-      </c>
-      <c r="C21">
-        <v>14798</v>
-      </c>
-      <c r="D21">
-        <v>7</v>
-      </c>
-      <c r="E21" t="s">
-        <v>55</v>
-      </c>
-      <c r="F21" t="s">
-        <v>907</v>
-      </c>
-      <c r="G21" t="s">
-        <v>914</v>
-      </c>
-      <c r="H21" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B22" s="1">
-        <v>43890</v>
-      </c>
-      <c r="C22">
-        <v>14802</v>
-      </c>
-      <c r="D22">
-        <v>7</v>
-      </c>
-      <c r="E22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" t="s">
-        <v>907</v>
-      </c>
-      <c r="G22" t="s">
-        <v>914</v>
-      </c>
-      <c r="H22" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>8</v>
-      </c>
-      <c r="B23" s="1">
-        <v>43861</v>
-      </c>
-      <c r="C23">
-        <v>11682</v>
-      </c>
-      <c r="D23">
-        <v>7</v>
-      </c>
-      <c r="E23" t="s">
-        <v>55</v>
-      </c>
-      <c r="F23" t="s">
-        <v>907</v>
-      </c>
-      <c r="G23" t="s">
-        <v>914</v>
-      </c>
-      <c r="H23" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="1">
-        <v>43921</v>
-      </c>
-      <c r="C24">
-        <v>458</v>
-      </c>
-      <c r="D24">
-        <v>7</v>
-      </c>
-      <c r="E24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F24" t="s">
-        <v>907</v>
-      </c>
-      <c r="G24" t="s">
-        <v>914</v>
-      </c>
-      <c r="H24" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>14</v>
-      </c>
-      <c r="B25" s="1">
-        <v>43890</v>
-      </c>
-      <c r="C25">
-        <v>508</v>
-      </c>
-      <c r="D25">
-        <v>7</v>
-      </c>
-      <c r="E25" t="s">
-        <v>55</v>
-      </c>
-      <c r="F25" t="s">
-        <v>907</v>
-      </c>
-      <c r="G25" t="s">
-        <v>914</v>
-      </c>
-      <c r="H25" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>14</v>
-      </c>
-      <c r="B26" s="1">
-        <v>43861</v>
-      </c>
-      <c r="C26">
-        <v>358</v>
-      </c>
-      <c r="D26">
-        <v>7</v>
-      </c>
-      <c r="E26" t="s">
-        <v>55</v>
-      </c>
-      <c r="F26" t="s">
-        <v>907</v>
-      </c>
-      <c r="G26" t="s">
-        <v>914</v>
-      </c>
-      <c r="H26" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>41</v>
-      </c>
-      <c r="B27" s="1">
-        <v>43921</v>
-      </c>
-      <c r="C27">
-        <v>1484</v>
-      </c>
-      <c r="D27">
-        <v>7</v>
-      </c>
-      <c r="E27" t="s">
-        <v>55</v>
-      </c>
-      <c r="F27" t="s">
-        <v>907</v>
-      </c>
-      <c r="G27" t="s">
-        <v>914</v>
-      </c>
-      <c r="H27" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>41</v>
-      </c>
-      <c r="B28" s="1">
-        <v>43890</v>
-      </c>
-      <c r="C28">
-        <v>1483</v>
-      </c>
-      <c r="D28">
-        <v>7</v>
-      </c>
-      <c r="E28" t="s">
-        <v>55</v>
-      </c>
-      <c r="F28" t="s">
-        <v>907</v>
-      </c>
-      <c r="G28" t="s">
-        <v>914</v>
-      </c>
-      <c r="H28" t="s">
-        <v>914</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" s="1">
-        <v>43861</v>
-      </c>
-      <c r="C29">
-        <v>1172</v>
-      </c>
-      <c r="D29">
-        <v>7</v>
-      </c>
-      <c r="E29" t="s">
-        <v>55</v>
-      </c>
-      <c r="F29" t="s">
-        <v>907</v>
-      </c>
-      <c r="G29" t="s">
-        <v>914</v>
-      </c>
-      <c r="H29" t="s">
-        <v>914</v>
+      <c r="C40" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B40,VolumebyClient[Quarter],Summary!C$36)</f>
+        <v>69053</v>
+      </c>
+      <c r="D40" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B40,VolumebyClient[Quarter],Summary!D$36)</f>
+        <v>82618</v>
+      </c>
+      <c r="E40" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B40,VolumebyClient[Quarter],Summary!E$36)</f>
+        <v>50574</v>
+      </c>
+      <c r="F40" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B40,VolumebyClient[Quarter],Summary!F$36)</f>
+        <v>65121</v>
+      </c>
+      <c r="G40" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B40,VolumebyClient[Quarter],Summary!G$36)</f>
+        <v>75265</v>
+      </c>
+      <c r="H40" s="5">
+        <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B40,VolumebyClient[Quarter],Summary!H$36)</f>
+        <v>82631</v>
+      </c>
+      <c r="J40" s="9">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="K40" s="45">
+        <f t="shared" si="1"/>
+        <v>1.5735069839495353E-4</v>
+      </c>
+      <c r="M40" s="9">
+        <f t="shared" si="2"/>
+        <v>6225</v>
+      </c>
+      <c r="N40" s="45">
+        <f t="shared" si="3"/>
+        <v>4.1042783393002047E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B41" s="19" t="s">
+        <v>945</v>
+      </c>
+      <c r="C41" s="36">
+        <f>SUM(C37:C40)</f>
+        <v>822060</v>
+      </c>
+      <c r="D41" s="36">
+        <f t="shared" ref="D41:H41" si="4">SUM(D37:D40)</f>
+        <v>940140</v>
+      </c>
+      <c r="E41" s="36">
+        <f t="shared" si="4"/>
+        <v>587002</v>
+      </c>
+      <c r="F41" s="36">
+        <f t="shared" si="4"/>
+        <v>706563</v>
+      </c>
+      <c r="G41" s="36">
+        <f t="shared" si="4"/>
+        <v>855266</v>
+      </c>
+      <c r="H41" s="36">
+        <f t="shared" si="4"/>
+        <v>965282</v>
+      </c>
+      <c r="J41" s="36">
+        <f t="shared" si="0"/>
+        <v>25142</v>
+      </c>
+      <c r="K41" s="46">
+        <f t="shared" si="1"/>
+        <v>2.6742825536622217E-2</v>
+      </c>
+      <c r="M41" s="36">
+        <f t="shared" si="2"/>
+        <v>58348</v>
+      </c>
+      <c r="N41" s="46">
+        <f t="shared" si="3"/>
+        <v>3.3110884122120154E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
+  <pageSetup paperSize="20" orientation="portrait" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="4" id="{B3D8EE3A-3A5E-4CF8-9DDE-42D85FC7756C}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>G21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="3" id="{CEE82153-BA13-47BE-9239-ACC0A04E6262}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>C21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="2" id="{E512727B-3884-4032-BCB0-D25858D03DC6}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>K37:K41</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="1" id="{1FD74CE5-4633-4699-8E34-6E38153DA2FA}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>N37:N41</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -25347,8 +25177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{472D7B1D-3022-458C-99D2-1C6B8FA100F0}">
   <dimension ref="A3:Y136"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="N72" sqref="N72"/>
+    <sheetView topLeftCell="G16" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -26241,7 +26071,9 @@
       <c r="P44"/>
       <c r="Q44"/>
       <c r="R44"/>
-      <c r="S44"/>
+      <c r="S44" s="22" t="s">
+        <v>950</v>
+      </c>
       <c r="T44"/>
       <c r="U44"/>
       <c r="V44"/>
@@ -28787,8 +28619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F047ED54-646C-4103-A593-3F0BE14E8786}">
   <dimension ref="A1:R908"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView topLeftCell="A815" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2:R7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Reformatting and Finalizing Key Notes
</commit_message>
<xml_diff>
--- a/Volume by Region Data Request v3.xlsx
+++ b/Volume by Region Data Request v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sahil\Documents\Github\excelprogress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDD813BE-A853-4677-A689-4EADCF75AB4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B85D030-863C-4918-84DD-57FDCF607B1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" tabRatio="458" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28440" tabRatio="458" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Email" sheetId="73" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3301" uniqueCount="964">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3306" uniqueCount="964">
   <si>
     <t>CLID</t>
   </si>
@@ -2929,18 +2929,6 @@
     <t>All data as of 2/10/2022</t>
   </si>
   <si>
-    <t>Number of Customers YOY</t>
-  </si>
-  <si>
-    <t>Volume YOY</t>
-  </si>
-  <si>
-    <t>Distribution by Region</t>
-  </si>
-  <si>
-    <t>Data With Variance</t>
-  </si>
-  <si>
     <t>Customers</t>
   </si>
   <si>
@@ -2960,6 +2948,18 @@
   </si>
   <si>
     <t>Q2 Customers</t>
+  </si>
+  <si>
+    <t>Key Notes :</t>
+  </si>
+  <si>
+    <t>Q2 YOY growth slowed from Q1 growth of 4% down to 2.7%, (~13k) in volume primarily driven by:</t>
+  </si>
+  <si>
+    <t>- (~7k) volume, or 55% of the total decline from loss of two customers in LATAM, driving overall growth for region down from 9% in Q1 to flat in Q2 YoY</t>
+  </si>
+  <si>
+    <t>- NAM client onboarding in Q2 2020 anniversaried in Q2 2021, slowing perceived growth and amplifying Q1 growth by ~5k units, or 1%</t>
   </si>
 </sst>
 </file>
@@ -2971,7 +2971,7 @@
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="0,&quot;k&quot;"/>
-    <numFmt numFmtId="170" formatCode="0.0%;\(0.0%\)"/>
+    <numFmt numFmtId="167" formatCode="0.0%;\(0.0%\)"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -3098,7 +3098,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
@@ -3187,9 +3187,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
@@ -3199,16 +3196,21 @@
     <xf numFmtId="9" fontId="6" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="170" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="4" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -3553,8 +3555,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.1186656015824112E-2"/>
-          <c:y val="0.13717972107986753"/>
+          <c:x val="2.2402017163584892E-2"/>
+          <c:y val="0.13717965330119458"/>
           <c:w val="0.60094637318062527"/>
           <c:h val="0.7396265769603646"/>
         </c:manualLayout>
@@ -3589,6 +3591,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-84CC-4062-8CF4-E583810A0592}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -3604,6 +3611,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-84CC-4062-8CF4-E583810A0592}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="2"/>
@@ -3619,6 +3631,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-84CC-4062-8CF4-E583810A0592}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="3"/>
@@ -3634,6 +3651,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-84CC-4062-8CF4-E583810A0592}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:numFmt formatCode="0,\k" sourceLinked="0"/>
@@ -3783,6 +3805,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000009-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="1"/>
@@ -3798,6 +3825,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{0000000B-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="2"/>
@@ -3813,6 +3845,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{0000000D-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="3"/>
@@ -3828,6 +3865,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{0000000F-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:cat>
                   <c:strRef>
@@ -3895,7 +3937,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$D$24</c15:sqref>
@@ -3924,6 +3966,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000011-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="1"/>
@@ -3939,6 +3986,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000013-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="2"/>
@@ -3954,6 +4006,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000015-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="3"/>
@@ -3969,10 +4026,15 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000017-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$B$25:$B$28</c15:sqref>
@@ -3998,7 +4060,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$D$25:$D$28</c15:sqref>
@@ -4023,7 +4085,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000001-DB0A-4165-A89D-0E98452E84BA}"/>
                   </c:ext>
@@ -4036,7 +4098,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$E$24</c15:sqref>
@@ -4065,6 +4127,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000019-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="1"/>
@@ -4080,6 +4147,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{0000001B-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="2"/>
@@ -4095,6 +4167,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{0000001D-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="3"/>
@@ -4110,10 +4187,15 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{0000001F-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$B$25:$B$28</c15:sqref>
@@ -4139,7 +4221,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$E$25:$E$28</c15:sqref>
@@ -4164,7 +4246,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-DB0A-4165-A89D-0E98452E84BA}"/>
                   </c:ext>
@@ -4177,7 +4259,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$F$24</c15:sqref>
@@ -4206,6 +4288,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000021-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="1"/>
@@ -4221,6 +4308,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000023-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="2"/>
@@ -4236,6 +4328,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000025-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="3"/>
@@ -4251,10 +4348,15 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000027-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$B$25:$B$28</c15:sqref>
@@ -4280,7 +4382,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$F$25:$F$28</c15:sqref>
@@ -4305,7 +4407,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-DB0A-4165-A89D-0E98452E84BA}"/>
                   </c:ext>
@@ -4318,7 +4420,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$G$24</c15:sqref>
@@ -4347,6 +4449,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{00000029-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="1"/>
@@ -4362,6 +4469,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{0000002B-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="2"/>
@@ -4377,6 +4489,11 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{0000002D-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:dPt>
                   <c:idx val="3"/>
@@ -4392,10 +4509,15 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
+                  <c:extLst>
+                    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                      <c16:uniqueId val="{0000002F-84CC-4062-8CF4-E583810A0592}"/>
+                    </c:ext>
+                  </c:extLst>
                 </c:dPt>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$B$25:$B$28</c15:sqref>
@@ -4421,7 +4543,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$G$25:$G$28</c15:sqref>
@@ -4446,7 +4568,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-DB0A-4165-A89D-0E98452E84BA}"/>
                   </c:ext>
@@ -4522,8 +4644,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.1186656015824112E-2"/>
-          <c:y val="0.13717972107986753"/>
+          <c:x val="0.11902427450805939"/>
+          <c:y val="0.13717965330119458"/>
           <c:w val="0.58579485802911002"/>
           <c:h val="0.72097855146689849"/>
         </c:manualLayout>
@@ -4904,7 +5026,7 @@
                 <c:order val="1"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$D$32</c15:sqref>
@@ -4933,7 +5055,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000013-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -4953,7 +5075,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000015-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -4973,7 +5095,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000017-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -4993,7 +5115,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000019-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -5001,7 +5123,7 @@
                 </c:dPt>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$B$33:$B$36</c15:sqref>
@@ -5027,7 +5149,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$D$33:$D$36</c15:sqref>
@@ -5052,7 +5174,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000001A-48F0-40C2-A87E-D0B1CB522DF1}"/>
                   </c:ext>
@@ -5065,7 +5187,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$E$32</c15:sqref>
@@ -5094,7 +5216,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{0000001C-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -5114,7 +5236,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{0000001E-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -5134,7 +5256,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000020-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -5154,7 +5276,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000022-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -5162,7 +5284,7 @@
                 </c:dPt>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$B$33:$B$36</c15:sqref>
@@ -5188,7 +5310,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$E$33:$E$36</c15:sqref>
@@ -5213,7 +5335,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000023-48F0-40C2-A87E-D0B1CB522DF1}"/>
                   </c:ext>
@@ -5226,7 +5348,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$F$32</c15:sqref>
@@ -5255,7 +5377,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000025-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -5275,7 +5397,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000027-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -5295,7 +5417,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000029-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -5315,7 +5437,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{0000002B-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -5323,7 +5445,7 @@
                 </c:dPt>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$B$33:$B$36</c15:sqref>
@@ -5349,7 +5471,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$F$33:$F$36</c15:sqref>
@@ -5374,7 +5496,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{0000002C-48F0-40C2-A87E-D0B1CB522DF1}"/>
                   </c:ext>
@@ -5387,7 +5509,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$G$32</c15:sqref>
@@ -5416,7 +5538,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{0000002E-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -5436,7 +5558,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000030-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -5456,7 +5578,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000032-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -5476,7 +5598,7 @@
                     </a:ln>
                     <a:effectLst/>
                   </c:spPr>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                       <c16:uniqueId val="{00000034-48F0-40C2-A87E-D0B1CB522DF1}"/>
                     </c:ext>
@@ -5484,7 +5606,7 @@
                 </c:dPt>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$B$33:$B$36</c15:sqref>
@@ -5510,7 +5632,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$G$33:$G$36</c15:sqref>
@@ -5535,7 +5657,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000035-48F0-40C2-A87E-D0B1CB522DF1}"/>
                   </c:ext>
@@ -6180,7 +6302,7 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$E$24</c15:sqref>
@@ -6207,7 +6329,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$B$25:$B$28</c15:sqref>
@@ -6233,7 +6355,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$E$25:$E$28</c15:sqref>
@@ -6258,7 +6380,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-640E-47A9-9243-65ACB7DCCC5E}"/>
                   </c:ext>
@@ -6271,7 +6393,7 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$F$24</c15:sqref>
@@ -6298,7 +6420,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$B$25:$B$28</c15:sqref>
@@ -6324,7 +6446,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$F$25:$F$28</c15:sqref>
@@ -6349,7 +6471,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000003-640E-47A9-9243-65ACB7DCCC5E}"/>
                   </c:ext>
@@ -6362,7 +6484,7 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$G$24</c15:sqref>
@@ -6389,7 +6511,7 @@
                 <c:invertIfNegative val="0"/>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$B$25:$B$28</c15:sqref>
@@ -6415,7 +6537,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>Summary!$G$25:$G$28</c15:sqref>
@@ -6440,7 +6562,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-640E-47A9-9243-65ACB7DCCC5E}"/>
                   </c:ext>
@@ -19428,6 +19550,657 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D37C5FD1-A12E-4EA3-A67C-2BFE15959C89}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" numFmtId="14" showAll="0" defaultSubtotal="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="4">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="5"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item sd="0" x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item sd="0" x="3"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="9"/>
+    <field x="8"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="5"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Vol" fld="2" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="12">
+    <format dxfId="41">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="40">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="39">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="38">
+      <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="37">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="36">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
+    </format>
+    <format dxfId="35">
+      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="34">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="5" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="33">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="32">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="9" count="2">
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="31">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="30">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="10">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B3596AE5-7ABE-4BFD-935E-B17364891890}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A33:G40" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField numFmtId="14" showAll="0" defaultSubtotal="0">
+      <items count="14">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" numFmtId="164" showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
+      <items count="4">
+        <item x="3"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="1"/>
+      </items>
+      <autoSortScope>
+        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
+          <references count="1">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </autoSortScope>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="6">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
+      <items count="4">
+        <item sd="0" x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item sd="0" x="3"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="5"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="2">
+    <field x="9"/>
+    <field x="8"/>
+  </colFields>
+  <colItems count="6">
+    <i>
+      <x v="1"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Vol" fld="2" baseField="0" baseItem="0" numFmtId="164"/>
+  </dataFields>
+  <formats count="12">
+    <format dxfId="53">
+      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="52">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="51">
+      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="50">
+      <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
+    </format>
+    <format dxfId="49">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
+    </format>
+    <format dxfId="48">
+      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0"/>
+    </format>
+    <format dxfId="47">
+      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="46">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="5" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="45">
+      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="44">
+      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
+        <references count="1">
+          <reference field="9" count="2">
+            <x v="1"/>
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="43">
+      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
+    </format>
+    <format dxfId="42">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <chartFormats count="10">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="2" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="3" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="4"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="4" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="5" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="3">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="8" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="9" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="6" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="3"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="7" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="8" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="9" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F97460C6-2B1D-4429-9AE1-5403229ACA8E}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="1">
   <location ref="A51:J111" firstHeaderRow="1" firstDataRow="3" firstDataCol="2"/>
   <pivotFields count="10">
@@ -19845,657 +20618,6 @@
     <dataField name="Sum of Vol" fld="2" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="12">
-    <format dxfId="41">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="40">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="39">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="38">
-      <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
-    </format>
-    <format dxfId="37">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
-    </format>
-    <format dxfId="36">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0"/>
-    </format>
-    <format dxfId="35">
-      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="34">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="5" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="33">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="32">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="9" count="2">
-            <x v="1"/>
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="31">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="30">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="10">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="9" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="9" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="9" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="9" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="9" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="9" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D37C5FD1-A12E-4EA3-A67C-2BFE15959C89}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" numFmtId="14" showAll="0" defaultSubtotal="0">
-      <items count="14">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="164" showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisCol" showAll="0" sortType="descending" defaultSubtotal="0">
-      <items count="4">
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item sd="0" x="0"/>
-        <item sd="0" x="1"/>
-        <item sd="0" x="2"/>
-        <item sd="0" x="3"/>
-        <item sd="0" x="4"/>
-        <item sd="0" x="5"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisRow" showAll="0" defaultSubtotal="0">
-      <items count="4">
-        <item sd="0" x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item sd="0" x="3"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="3">
-    <field x="9"/>
-    <field x="8"/>
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="5"/>
-  </colFields>
-  <colItems count="4">
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Vol" fld="2" baseField="0" baseItem="0" numFmtId="164"/>
-  </dataFields>
-  <formats count="12">
-    <format dxfId="53">
-      <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="52">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-    <format dxfId="51">
-      <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="50">
-      <pivotArea field="9" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
-    </format>
-    <format dxfId="49">
-      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
-    <format dxfId="48">
-      <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="2"/>
-    </format>
-    <format dxfId="47">
-      <pivotArea field="5" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
-    </format>
-    <format dxfId="46">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="5" count="0"/>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="45">
-      <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="44">
-      <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
-        <references count="1">
-          <reference field="9" count="2">
-            <x v="1"/>
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-    <format dxfId="43">
-      <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
-    </format>
-    <format dxfId="42">
-      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
-    </format>
-  </formats>
-  <chartFormats count="10">
-    <chartFormat chart="0" format="0" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="9" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="1" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="9" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-          <reference field="9" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="3" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="4"/>
-          </reference>
-          <reference field="9" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="4" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-          <reference field="9" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="5" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="8" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="9" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="6" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="3"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="7" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="8" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="9" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="5" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-  </chartFormats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B3596AE5-7ABE-4BFD-935E-B17364891890}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="7" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="7" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A33:G40" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField numFmtId="14" showAll="0" defaultSubtotal="0">
-      <items count="14">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item x="12"/>
-        <item x="13"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" numFmtId="164" showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisRow" showAll="0" sortType="descending" defaultSubtotal="0">
-      <items count="4">
-        <item x="3"/>
-        <item x="2"/>
-        <item x="0"/>
-        <item x="1"/>
-      </items>
-      <autoSortScope>
-        <pivotArea dataOnly="0" outline="0" fieldPosition="0">
-          <references count="1">
-            <reference field="4294967294" count="1" selected="0">
-              <x v="0"/>
-            </reference>
-          </references>
-        </pivotArea>
-      </autoSortScope>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0" defaultSubtotal="0"/>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="6">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-      </items>
-    </pivotField>
-    <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
-      <items count="4">
-        <item sd="0" x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item sd="0" x="3"/>
-      </items>
-    </pivotField>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="5"/>
-  </rowFields>
-  <rowItems count="5">
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="2">
-    <field x="9"/>
-    <field x="8"/>
-  </colFields>
-  <colItems count="6">
-    <i>
-      <x v="1"/>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-    <i r="1">
-      <x v="3"/>
-    </i>
-    <i r="1">
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="2"/>
-      <x v="1"/>
-    </i>
-    <i r="1">
-      <x v="2"/>
-    </i>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Vol" fld="2" baseField="0" baseItem="0" numFmtId="164"/>
-  </dataFields>
-  <formats count="12">
     <format dxfId="65">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
@@ -20687,10 +20809,10 @@
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" fillDownLabelsDefault="1" hideValuesRow="1"/>
     </ext>
     <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16 EnabledSubtotalsDefault="0" SubtotalsOnTopDefault="0"/>
+      <xpdl:pivotTableDefinition16/>
     </ext>
   </extLst>
 </pivotTableDefinition>
@@ -21109,150 +21231,150 @@
   <sheetFormatPr defaultRowHeight="13.15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="49" t="s">
         <v>897</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
     </row>
     <row r="2" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="40"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
     </row>
     <row r="3" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
+      <c r="A3" s="49"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
     </row>
     <row r="4" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
+      <c r="A4" s="49"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
     </row>
     <row r="5" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="40"/>
-      <c r="B5" s="40"/>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
-      <c r="G5" s="40"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
     </row>
     <row r="6" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="40"/>
-      <c r="B6" s="40"/>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
-      <c r="G6" s="40"/>
+      <c r="A6" s="49"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
     </row>
     <row r="7" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="40"/>
-      <c r="B7" s="40"/>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
+      <c r="A7" s="49"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
     </row>
     <row r="8" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="40"/>
-      <c r="B8" s="40"/>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
+      <c r="A8" s="49"/>
+      <c r="B8" s="49"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
     </row>
     <row r="9" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="40"/>
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
+      <c r="A9" s="49"/>
+      <c r="B9" s="49"/>
+      <c r="C9" s="49"/>
+      <c r="D9" s="49"/>
+      <c r="E9" s="49"/>
+      <c r="F9" s="49"/>
+      <c r="G9" s="49"/>
     </row>
     <row r="10" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="40"/>
-      <c r="B10" s="40"/>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
+      <c r="A10" s="49"/>
+      <c r="B10" s="49"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
     </row>
     <row r="11" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="40"/>
-      <c r="B11" s="40"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
+      <c r="A11" s="49"/>
+      <c r="B11" s="49"/>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49"/>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
     </row>
     <row r="12" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="40"/>
-      <c r="B12" s="40"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="40"/>
-      <c r="F12" s="40"/>
-      <c r="G12" s="40"/>
+      <c r="A12" s="49"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
     </row>
     <row r="13" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="40"/>
-      <c r="B13" s="40"/>
-      <c r="C13" s="40"/>
-      <c r="D13" s="40"/>
-      <c r="E13" s="40"/>
-      <c r="F13" s="40"/>
-      <c r="G13" s="40"/>
+      <c r="A13" s="49"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
     </row>
     <row r="14" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="40"/>
-      <c r="B14" s="40"/>
-      <c r="C14" s="40"/>
-      <c r="D14" s="40"/>
-      <c r="E14" s="40"/>
-      <c r="F14" s="40"/>
-      <c r="G14" s="40"/>
+      <c r="A14" s="49"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+      <c r="F14" s="49"/>
+      <c r="G14" s="49"/>
     </row>
     <row r="15" spans="1:7" ht="13.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="40"/>
-      <c r="B15" s="40"/>
-      <c r="C15" s="40"/>
-      <c r="D15" s="40"/>
-      <c r="E15" s="40"/>
-      <c r="F15" s="40"/>
-      <c r="G15" s="40"/>
+      <c r="A15" s="49"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="49"/>
+      <c r="D15" s="49"/>
+      <c r="E15" s="49"/>
+      <c r="F15" s="49"/>
+      <c r="G15" s="49"/>
     </row>
     <row r="16" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
-      <c r="C16" s="40"/>
-      <c r="D16" s="40"/>
-      <c r="E16" s="40"/>
-      <c r="F16" s="40"/>
-      <c r="G16" s="40"/>
+      <c r="A16" s="49"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="49"/>
+      <c r="E16" s="49"/>
+      <c r="F16" s="49"/>
+      <c r="G16" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -29564,15 +29686,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45F675FF-8571-44E8-8591-11391A021DF3}">
-  <dimension ref="B1:N60"/>
+  <dimension ref="B1:Q58"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="10.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="3"/>
@@ -29582,56 +29704,59 @@
     <col min="9" max="9" width="4.42578125" style="3" customWidth="1"/>
     <col min="10" max="11" width="9.140625" style="3"/>
     <col min="12" max="12" width="4.42578125" style="3" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="3"/>
+    <col min="13" max="13" width="11.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="3"/>
+    <col min="15" max="15" width="4.42578125" style="3" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="35.25" x14ac:dyDescent="0.5">
-      <c r="B1" s="46" t="s">
+    <row r="1" spans="2:7" ht="35.25" x14ac:dyDescent="0.5">
+      <c r="B1" s="45" t="s">
         <v>951</v>
       </c>
     </row>
-    <row r="2" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B2" s="47" t="s">
+    <row r="2" spans="2:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="B2" s="46" t="s">
         <v>952</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="20.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" ht="20.25" x14ac:dyDescent="0.2">
       <c r="B4" s="27" t="s">
-        <v>962</v>
+        <v>958</v>
       </c>
       <c r="C4" s="24"/>
-      <c r="E4" s="27" t="s">
-        <v>963</v>
-      </c>
-      <c r="F4" s="24"/>
-    </row>
-    <row r="5" spans="2:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="F4" s="27" t="s">
+        <v>959</v>
+      </c>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="2:7" ht="30" x14ac:dyDescent="0.2">
       <c r="B5" s="29">
         <f>H29</f>
         <v>965282</v>
       </c>
       <c r="C5" s="28"/>
-      <c r="E5" s="41">
+      <c r="F5" s="40">
         <f>H37</f>
         <v>50</v>
       </c>
-      <c r="F5" s="28"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="28"/>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B6" s="26" t="s">
-        <v>958</v>
+        <v>954</v>
       </c>
       <c r="C6" s="25" t="s">
-        <v>959</v>
-      </c>
-      <c r="E6" s="26" t="s">
-        <v>958</v>
-      </c>
-      <c r="F6" s="25" t="s">
-        <v>959</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+        <v>955</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>954</v>
+      </c>
+      <c r="G6" s="25" t="s">
+        <v>955</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B7" s="30">
         <f>D29</f>
         <v>940140</v>
@@ -29640,23 +29765,23 @@
         <f>B5/B7-1</f>
         <v>2.6742825536622217E-2</v>
       </c>
-      <c r="E7" s="42">
+      <c r="F7" s="41">
         <f>D37</f>
         <v>50</v>
       </c>
-      <c r="F7" s="43">
-        <f>E5/E7-1</f>
+      <c r="G7" s="42">
+        <f>F5/F7-1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="2:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="2:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="2:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="2:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="2:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="2:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="2:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" spans="2:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B23" s="33" t="s">
         <v>906</v>
       </c>
@@ -29667,15 +29792,19 @@
       <c r="G23" s="34"/>
       <c r="H23" s="34"/>
       <c r="J23" s="35" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="K23" s="36"/>
       <c r="M23" s="35" t="s">
-        <v>960</v>
+        <v>935</v>
       </c>
       <c r="N23" s="36"/>
-    </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="P23" s="35" t="s">
+        <v>956</v>
+      </c>
+      <c r="Q23" s="36"/>
+    </row>
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24" s="37" t="s">
         <v>921</v>
       </c>
@@ -29709,8 +29838,14 @@
       <c r="N24" s="39" t="s">
         <v>934</v>
       </c>
-    </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="P24" s="39" t="s">
+        <v>933</v>
+      </c>
+      <c r="Q24" s="39" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" s="20" t="s">
         <v>898</v>
       </c>
@@ -29734,28 +29869,36 @@
         <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B25,VolumebyClient[Quarter],Summary!G$24)</f>
         <v>530019</v>
       </c>
-      <c r="H25" s="48">
+      <c r="H25" s="47">
         <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B25,VolumebyClient[Quarter],Summary!H$24)</f>
         <v>596502</v>
       </c>
       <c r="J25" s="9">
+        <f>G25-C25</f>
+        <v>20600</v>
+      </c>
+      <c r="K25" s="43">
+        <f>G25/C25-1</f>
+        <v>4.0438224722674221E-2</v>
+      </c>
+      <c r="M25" s="9">
         <f>H25-D25</f>
         <v>19884</v>
       </c>
-      <c r="K25" s="44">
+      <c r="N25" s="43">
         <f>H25/D25-1</f>
         <v>3.4483835051975387E-2</v>
       </c>
-      <c r="M25" s="9">
+      <c r="P25" s="9">
         <f>SUM(G25:H25)-SUM(C25:D25)</f>
         <v>40484</v>
       </c>
-      <c r="N25" s="44">
+      <c r="Q25" s="43">
         <f>SUM(G25:H25)/SUM(C25:D25)-1</f>
         <v>3.7276814694158666E-2</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B26" s="20" t="s">
         <v>899</v>
       </c>
@@ -29779,28 +29922,36 @@
         <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B26,VolumebyClient[Quarter],Summary!G$24)</f>
         <v>150204</v>
       </c>
-      <c r="H26" s="48">
+      <c r="H26" s="47">
         <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B26,VolumebyClient[Quarter],Summary!H$24)</f>
         <v>176338</v>
       </c>
       <c r="J26" s="9">
-        <f t="shared" ref="J26:J29" si="0">H26-D26</f>
+        <f t="shared" ref="J26:J29" si="0">G26-C26</f>
+        <v>2352</v>
+      </c>
+      <c r="K26" s="43">
+        <f t="shared" ref="K26:K29" si="1">G26/C26-1</f>
+        <v>1.5907799691583513E-2</v>
+      </c>
+      <c r="M26" s="9">
+        <f>H26-D26</f>
         <v>2772</v>
       </c>
-      <c r="K26" s="44">
-        <f t="shared" ref="K26:K29" si="1">H26/D26-1</f>
+      <c r="N26" s="43">
+        <f>H26/D26-1</f>
         <v>1.5970869870827187E-2</v>
       </c>
-      <c r="M26" s="9">
-        <f t="shared" ref="M26:M29" si="2">SUM(G26:H26)-SUM(C26:D26)</f>
+      <c r="P26" s="9">
+        <f>SUM(G26:H26)-SUM(C26:D26)</f>
         <v>5124</v>
       </c>
-      <c r="N26" s="44">
-        <f t="shared" ref="N26:N29" si="3">SUM(G26:H26)/SUM(C26:D26)-1</f>
+      <c r="Q26" s="43">
+        <f>SUM(G26:H26)/SUM(C26:D26)-1</f>
         <v>1.5941857643318125E-2</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" s="20" t="s">
         <v>908</v>
       </c>
@@ -29824,28 +29975,36 @@
         <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B27,VolumebyClient[Quarter],Summary!G$24)</f>
         <v>99778</v>
       </c>
-      <c r="H27" s="48">
+      <c r="H27" s="47">
         <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B27,VolumebyClient[Quarter],Summary!H$24)</f>
         <v>109811</v>
       </c>
       <c r="J27" s="9">
         <f t="shared" si="0"/>
+        <v>4042</v>
+      </c>
+      <c r="K27" s="43">
+        <f t="shared" si="1"/>
+        <v>4.2220272415810056E-2</v>
+      </c>
+      <c r="M27" s="9">
+        <f>H27-D27</f>
         <v>2473</v>
       </c>
-      <c r="K27" s="44">
-        <f t="shared" si="1"/>
+      <c r="N27" s="43">
+        <f>H27/D27-1</f>
         <v>2.3039370959026639E-2</v>
       </c>
-      <c r="M27" s="9">
-        <f t="shared" si="2"/>
+      <c r="P27" s="9">
+        <f>SUM(G27:H27)-SUM(C27:D27)</f>
         <v>6515</v>
       </c>
-      <c r="N27" s="44">
-        <f t="shared" si="3"/>
+      <c r="Q27" s="43">
+        <f>SUM(G27:H27)/SUM(C27:D27)-1</f>
         <v>3.2081901178880656E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" s="20" t="s">
         <v>907</v>
       </c>
@@ -29869,28 +30028,36 @@
         <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B28,VolumebyClient[Quarter],Summary!G$24)</f>
         <v>75265</v>
       </c>
-      <c r="H28" s="48">
+      <c r="H28" s="47">
         <f>SUMIFS(VolumebyClient[Vol],VolumebyClient[Region Name],Summary!$B28,VolumebyClient[Quarter],Summary!H$24)</f>
         <v>82631</v>
       </c>
       <c r="J28" s="9">
         <f t="shared" si="0"/>
+        <v>6212</v>
+      </c>
+      <c r="K28" s="43">
+        <f t="shared" si="1"/>
+        <v>8.9959885884755231E-2</v>
+      </c>
+      <c r="M28" s="9">
+        <f>H28-D28</f>
         <v>13</v>
       </c>
-      <c r="K28" s="44">
-        <f t="shared" si="1"/>
+      <c r="N28" s="43">
+        <f>H28/D28-1</f>
         <v>1.5735069839495353E-4</v>
       </c>
-      <c r="M28" s="9">
-        <f t="shared" si="2"/>
+      <c r="P28" s="9">
+        <f>SUM(G28:H28)-SUM(C28:D28)</f>
         <v>6225</v>
       </c>
-      <c r="N28" s="44">
-        <f t="shared" si="3"/>
+      <c r="Q28" s="43">
+        <f>SUM(G28:H28)/SUM(C28:D28)-1</f>
         <v>4.1042783393002047E-2</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B29" s="19" t="s">
         <v>945</v>
       </c>
@@ -29899,45 +30066,53 @@
         <v>822060</v>
       </c>
       <c r="D29" s="31">
-        <f t="shared" ref="D29:H29" si="4">SUM(D25:D28)</f>
+        <f t="shared" ref="D29:H29" si="2">SUM(D25:D28)</f>
         <v>940140</v>
       </c>
       <c r="E29" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>587002</v>
       </c>
       <c r="F29" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>706563</v>
       </c>
       <c r="G29" s="31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>855266</v>
       </c>
-      <c r="H29" s="49">
-        <f t="shared" si="4"/>
+      <c r="H29" s="48">
+        <f t="shared" si="2"/>
         <v>965282</v>
       </c>
       <c r="J29" s="31">
         <f t="shared" si="0"/>
+        <v>33206</v>
+      </c>
+      <c r="K29" s="44">
+        <f t="shared" si="1"/>
+        <v>4.0393645232708053E-2</v>
+      </c>
+      <c r="M29" s="31">
+        <f>H29-D29</f>
         <v>25142</v>
       </c>
-      <c r="K29" s="45">
-        <f t="shared" si="1"/>
+      <c r="N29" s="44">
+        <f>H29/D29-1</f>
         <v>2.6742825536622217E-2</v>
       </c>
-      <c r="M29" s="31">
-        <f t="shared" si="2"/>
+      <c r="P29" s="31">
+        <f>SUM(G29:H29)-SUM(C29:D29)</f>
         <v>58348</v>
       </c>
-      <c r="N29" s="45">
-        <f t="shared" si="3"/>
+      <c r="Q29" s="44">
+        <f>SUM(G29:H29)/SUM(C29:D29)-1</f>
         <v>3.3110884122120154E-2</v>
       </c>
     </row>
-    <row r="31" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B31" s="33" t="s">
-        <v>957</v>
+        <v>953</v>
       </c>
       <c r="C31" s="34"/>
       <c r="D31" s="34"/>
@@ -29946,15 +30121,19 @@
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
       <c r="J31" s="35" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="K31" s="36"/>
       <c r="M31" s="35" t="s">
-        <v>960</v>
+        <v>935</v>
       </c>
       <c r="N31" s="36"/>
-    </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="P31" s="35" t="s">
+        <v>956</v>
+      </c>
+      <c r="Q31" s="36"/>
+    </row>
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B32" s="37" t="s">
         <v>921</v>
       </c>
@@ -29988,8 +30167,14 @@
       <c r="N32" s="39" t="s">
         <v>934</v>
       </c>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="P32" s="39" t="s">
+        <v>933</v>
+      </c>
+      <c r="Q32" s="39" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B33" s="20" t="s">
         <v>898</v>
       </c>
@@ -30013,28 +30198,36 @@
         <f>ROUNDUP(COUNTIFS(VolumebyClient[Region Name],Summary!$B33,VolumebyClient[Quarter],Summary!G$32)/3,0)</f>
         <v>20</v>
       </c>
-      <c r="H33" s="48">
+      <c r="H33" s="47">
         <f>ROUNDUP(COUNTIFS(VolumebyClient[Region Name],Summary!$B33,VolumebyClient[Quarter],Summary!H$32)/3,0)</f>
         <v>20</v>
       </c>
       <c r="J33" s="9">
+        <f>G33-C33</f>
+        <v>2</v>
+      </c>
+      <c r="K33" s="43">
+        <f>G33/C33-1</f>
+        <v>0.11111111111111116</v>
+      </c>
+      <c r="M33" s="9">
         <f>H33-D33</f>
         <v>1</v>
       </c>
-      <c r="K33" s="44">
+      <c r="N33" s="43">
         <f>H33/D33-1</f>
         <v>5.2631578947368363E-2</v>
       </c>
-      <c r="M33" s="9">
+      <c r="P33" s="9">
         <f>SUM(G33:H33)-SUM(C33:D33)</f>
         <v>3</v>
       </c>
-      <c r="N33" s="44">
+      <c r="Q33" s="43">
         <f>SUM(G33:H33)/SUM(C33:D33)-1</f>
         <v>8.1081081081081141E-2</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B34" s="20" t="s">
         <v>899</v>
       </c>
@@ -30058,28 +30251,36 @@
         <f>ROUNDUP(COUNTIFS(VolumebyClient[Region Name],Summary!$B34,VolumebyClient[Quarter],Summary!G$32)/3,0)</f>
         <v>8</v>
       </c>
-      <c r="H34" s="48">
+      <c r="H34" s="47">
         <f>ROUNDUP(COUNTIFS(VolumebyClient[Region Name],Summary!$B34,VolumebyClient[Quarter],Summary!H$32)/3,0)</f>
         <v>8</v>
       </c>
       <c r="J34" s="9">
-        <f t="shared" ref="J34:J37" si="5">H34-D34</f>
+        <f t="shared" ref="J34:J37" si="3">G34-C34</f>
         <v>0</v>
       </c>
-      <c r="K34" s="44">
-        <f t="shared" ref="K34:K37" si="6">H34/D34-1</f>
+      <c r="K34" s="43">
+        <f t="shared" ref="K34:K37" si="4">G34/C34-1</f>
         <v>0</v>
       </c>
       <c r="M34" s="9">
-        <f t="shared" ref="M34:M37" si="7">SUM(G34:H34)-SUM(C34:D34)</f>
+        <f>H34-D34</f>
         <v>0</v>
       </c>
-      <c r="N34" s="44">
-        <f t="shared" ref="N34:N37" si="8">SUM(G34:H34)/SUM(C34:D34)-1</f>
+      <c r="N34" s="43">
+        <f>H34/D34-1</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="P34" s="9">
+        <f>SUM(G34:H34)-SUM(C34:D34)</f>
+        <v>0</v>
+      </c>
+      <c r="Q34" s="43">
+        <f>SUM(G34:H34)/SUM(C34:D34)-1</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B35" s="20" t="s">
         <v>908</v>
       </c>
@@ -30103,28 +30304,36 @@
         <f>ROUNDUP(COUNTIFS(VolumebyClient[Region Name],Summary!$B35,VolumebyClient[Quarter],Summary!G$32)/3,0)</f>
         <v>14</v>
       </c>
-      <c r="H35" s="48">
+      <c r="H35" s="47">
         <f>ROUNDUP(COUNTIFS(VolumebyClient[Region Name],Summary!$B35,VolumebyClient[Quarter],Summary!H$32)/3,0)</f>
         <v>13</v>
       </c>
       <c r="J35" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K35" s="43">
+        <f t="shared" si="4"/>
+        <v>7.6923076923076872E-2</v>
+      </c>
+      <c r="M35" s="9">
+        <f>H35-D35</f>
         <v>0</v>
       </c>
-      <c r="K35" s="44">
-        <f t="shared" si="6"/>
+      <c r="N35" s="43">
+        <f>H35/D35-1</f>
         <v>0</v>
       </c>
-      <c r="M35" s="9">
-        <f t="shared" si="7"/>
+      <c r="P35" s="9">
+        <f>SUM(G35:H35)-SUM(C35:D35)</f>
         <v>1</v>
       </c>
-      <c r="N35" s="44">
-        <f t="shared" si="8"/>
+      <c r="Q35" s="43">
+        <f>SUM(G35:H35)/SUM(C35:D35)-1</f>
         <v>3.8461538461538547E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B36" s="20" t="s">
         <v>907</v>
       </c>
@@ -30148,28 +30357,36 @@
         <f>ROUNDUP(COUNTIFS(VolumebyClient[Region Name],Summary!$B36,VolumebyClient[Quarter],Summary!G$32)/3,0)</f>
         <v>11</v>
       </c>
-      <c r="H36" s="48">
+      <c r="H36" s="47">
         <f>ROUNDUP(COUNTIFS(VolumebyClient[Region Name],Summary!$B36,VolumebyClient[Quarter],Summary!H$32)/3,0)</f>
         <v>9</v>
       </c>
       <c r="J36" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="K36" s="43">
+        <f t="shared" si="4"/>
+        <v>0.10000000000000009</v>
+      </c>
+      <c r="M36" s="9">
+        <f>H36-D36</f>
         <v>-1</v>
       </c>
-      <c r="K36" s="44">
-        <f t="shared" si="6"/>
+      <c r="N36" s="43">
+        <f>H36/D36-1</f>
         <v>-9.9999999999999978E-2</v>
       </c>
-      <c r="M36" s="9">
-        <f t="shared" si="7"/>
+      <c r="P36" s="9">
+        <f>SUM(G36:H36)-SUM(C36:D36)</f>
         <v>0</v>
       </c>
-      <c r="N36" s="44">
-        <f t="shared" si="8"/>
+      <c r="Q36" s="43">
+        <f>SUM(G36:H36)/SUM(C36:D36)-1</f>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B37" s="19" t="s">
         <v>945</v>
       </c>
@@ -30178,45 +30395,53 @@
         <v>49</v>
       </c>
       <c r="D37" s="31">
-        <f t="shared" ref="D37:H37" si="9">SUM(D33:D36)</f>
+        <f t="shared" ref="D37:H37" si="5">SUM(D33:D36)</f>
         <v>50</v>
       </c>
       <c r="E37" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>52</v>
       </c>
       <c r="F37" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>53</v>
       </c>
       <c r="G37" s="31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="5"/>
         <v>53</v>
       </c>
-      <c r="H37" s="49">
-        <f t="shared" si="9"/>
+      <c r="H37" s="48">
+        <f t="shared" si="5"/>
         <v>50</v>
       </c>
       <c r="J37" s="31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="K37" s="44">
+        <f t="shared" si="4"/>
+        <v>8.163265306122458E-2</v>
+      </c>
+      <c r="M37" s="31">
+        <f>H37-D37</f>
         <v>0</v>
       </c>
-      <c r="K37" s="45">
-        <f t="shared" si="6"/>
+      <c r="N37" s="44">
+        <f>H37/D37-1</f>
         <v>0</v>
       </c>
-      <c r="M37" s="31">
-        <f t="shared" si="7"/>
+      <c r="P37" s="31">
+        <f>SUM(G37:H37)-SUM(C37:D37)</f>
         <v>4</v>
       </c>
-      <c r="N37" s="45">
-        <f t="shared" si="8"/>
+      <c r="Q37" s="44">
+        <f>SUM(G37:H37)/SUM(C37:D37)-1</f>
         <v>4.0404040404040442E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:14" ht="15" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B39" s="33" t="s">
-        <v>961</v>
+        <v>957</v>
       </c>
       <c r="C39" s="34"/>
       <c r="D39" s="34"/>
@@ -30225,15 +30450,19 @@
       <c r="G39" s="34"/>
       <c r="H39" s="34"/>
       <c r="J39" s="35" t="s">
-        <v>935</v>
+        <v>932</v>
       </c>
       <c r="K39" s="36"/>
       <c r="M39" s="35" t="s">
-        <v>960</v>
+        <v>935</v>
       </c>
       <c r="N39" s="36"/>
-    </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="P39" s="35" t="s">
+        <v>956</v>
+      </c>
+      <c r="Q39" s="36"/>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B40" s="37" t="s">
         <v>921</v>
       </c>
@@ -30267,8 +30496,14 @@
       <c r="N40" s="39" t="s">
         <v>934</v>
       </c>
-    </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="P40" s="39" t="s">
+        <v>933</v>
+      </c>
+      <c r="Q40" s="39" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B41" s="20" t="s">
         <v>898</v>
       </c>
@@ -30277,261 +30512,297 @@
         <v>28301.055555555555</v>
       </c>
       <c r="D41" s="5">
-        <f t="shared" ref="D41:H41" si="10">D25/D33</f>
+        <f t="shared" ref="D41:H41" si="6">D25/D33</f>
         <v>30348.315789473683</v>
       </c>
       <c r="E41" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>19141.78947368421</v>
       </c>
       <c r="F41" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>21601.7</v>
       </c>
       <c r="G41" s="5">
-        <f t="shared" si="10"/>
+        <f t="shared" si="6"/>
         <v>26500.95</v>
       </c>
-      <c r="H41" s="48">
-        <f t="shared" si="10"/>
+      <c r="H41" s="47">
+        <f t="shared" si="6"/>
         <v>29825.1</v>
       </c>
       <c r="J41" s="9">
+        <f>G41-C41</f>
+        <v>-1800.105555555554</v>
+      </c>
+      <c r="K41" s="43">
+        <f>G41/C41-1</f>
+        <v>-6.3605597749593068E-2</v>
+      </c>
+      <c r="M41" s="9">
         <f>H41-D41</f>
         <v>-523.21578947368471</v>
       </c>
-      <c r="K41" s="44">
+      <c r="N41" s="43">
         <f>H41/D41-1</f>
         <v>-1.7240356700623294E-2</v>
       </c>
-      <c r="M41" s="9">
+      <c r="P41" s="9">
         <f>SUM(G41:H41)-SUM(C41:D41)</f>
         <v>-2323.3213450292387</v>
       </c>
-      <c r="N41" s="44">
+      <c r="Q41" s="43">
         <f>SUM(G41:H41)/SUM(C41:D41)-1</f>
         <v>-3.9613746775925995E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B42" s="20" t="s">
         <v>899</v>
       </c>
       <c r="C42" s="5">
-        <f t="shared" ref="C42:H42" si="11">C26/C34</f>
+        <f t="shared" ref="C42:H42" si="7">C26/C34</f>
         <v>18481.5</v>
       </c>
       <c r="D42" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>21695.75</v>
       </c>
       <c r="E42" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>12942</v>
       </c>
       <c r="F42" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>16158</v>
       </c>
       <c r="G42" s="5">
-        <f t="shared" si="11"/>
+        <f t="shared" si="7"/>
         <v>18775.5</v>
       </c>
-      <c r="H42" s="48">
-        <f t="shared" si="11"/>
+      <c r="H42" s="47">
+        <f t="shared" si="7"/>
         <v>22042.25</v>
       </c>
       <c r="J42" s="9">
-        <f t="shared" ref="J42:J45" si="12">H42-D42</f>
+        <f t="shared" ref="J42:J45" si="8">G42-C42</f>
+        <v>294</v>
+      </c>
+      <c r="K42" s="43">
+        <f t="shared" ref="K42:K45" si="9">G42/C42-1</f>
+        <v>1.5907799691583513E-2</v>
+      </c>
+      <c r="M42" s="9">
+        <f>H42-D42</f>
         <v>346.5</v>
       </c>
-      <c r="K42" s="44">
-        <f t="shared" ref="K42:K45" si="13">H42/D42-1</f>
+      <c r="N42" s="43">
+        <f>H42/D42-1</f>
         <v>1.5970869870827187E-2</v>
       </c>
-      <c r="M42" s="9">
-        <f t="shared" ref="M42:M45" si="14">SUM(G42:H42)-SUM(C42:D42)</f>
+      <c r="P42" s="9">
+        <f>SUM(G42:H42)-SUM(C42:D42)</f>
         <v>640.5</v>
       </c>
-      <c r="N42" s="44">
-        <f t="shared" ref="N42:N45" si="15">SUM(G42:H42)/SUM(C42:D42)-1</f>
+      <c r="Q42" s="43">
+        <f>SUM(G42:H42)/SUM(C42:D42)-1</f>
         <v>1.5941857643318125E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B43" s="20" t="s">
         <v>908</v>
       </c>
       <c r="C43" s="5">
-        <f t="shared" ref="C43:H43" si="16">C27/C35</f>
+        <f t="shared" ref="C43:H43" si="10">C27/C35</f>
         <v>7364.3076923076924</v>
       </c>
       <c r="D43" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>8256.7692307692305</v>
       </c>
       <c r="E43" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>4942.7142857142853</v>
       </c>
       <c r="F43" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>5724.5714285714284</v>
       </c>
       <c r="G43" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="10"/>
         <v>7127</v>
       </c>
-      <c r="H43" s="48">
-        <f t="shared" si="16"/>
+      <c r="H43" s="47">
+        <f t="shared" si="10"/>
         <v>8447</v>
       </c>
       <c r="J43" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
+        <v>-237.30769230769238</v>
+      </c>
+      <c r="K43" s="43">
+        <f t="shared" si="9"/>
+        <v>-3.2224032756747678E-2</v>
+      </c>
+      <c r="M43" s="9">
+        <f>H43-D43</f>
         <v>190.23076923076951</v>
       </c>
-      <c r="K43" s="44">
-        <f t="shared" si="13"/>
+      <c r="N43" s="43">
+        <f>H43/D43-1</f>
         <v>2.3039370959026639E-2</v>
       </c>
-      <c r="M43" s="9">
-        <f t="shared" si="14"/>
+      <c r="P43" s="9">
+        <f>SUM(G43:H43)-SUM(C43:D43)</f>
         <v>-47.076923076921958</v>
       </c>
-      <c r="N43" s="44">
-        <f t="shared" si="15"/>
+      <c r="Q43" s="43">
+        <f>SUM(G43:H43)/SUM(C43:D43)-1</f>
         <v>-3.0136797423598871E-3</v>
       </c>
     </row>
-    <row r="44" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B44" s="20" t="s">
         <v>907</v>
       </c>
       <c r="C44" s="5">
-        <f t="shared" ref="C44:H44" si="17">C28/C36</f>
+        <f t="shared" ref="C44:H44" si="11">C28/C36</f>
         <v>6905.3</v>
       </c>
       <c r="D44" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>8261.7999999999993</v>
       </c>
       <c r="E44" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>4597.636363636364</v>
       </c>
       <c r="F44" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>5920.090909090909</v>
       </c>
       <c r="G44" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="11"/>
         <v>6842.272727272727</v>
       </c>
-      <c r="H44" s="48">
-        <f t="shared" si="17"/>
+      <c r="H44" s="47">
+        <f t="shared" si="11"/>
         <v>9181.2222222222226</v>
       </c>
       <c r="J44" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
+        <v>-63.027272727273157</v>
+      </c>
+      <c r="K44" s="43">
+        <f t="shared" si="9"/>
+        <v>-9.1273764684044467E-3</v>
+      </c>
+      <c r="M44" s="9">
+        <f>H44-D44</f>
         <v>919.42222222222335</v>
       </c>
-      <c r="K44" s="44">
-        <f t="shared" si="13"/>
+      <c r="N44" s="43">
+        <f>H44/D44-1</f>
         <v>0.11128594522043911</v>
       </c>
-      <c r="M44" s="9">
-        <f t="shared" si="14"/>
+      <c r="P44" s="9">
+        <f>SUM(G44:H44)-SUM(C44:D44)</f>
         <v>856.39494949495202</v>
       </c>
-      <c r="N44" s="44">
-        <f t="shared" si="15"/>
+      <c r="Q44" s="43">
+        <f>SUM(G44:H44)/SUM(C44:D44)-1</f>
         <v>5.6463987808806682E-2</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B45" s="19" t="s">
         <v>945</v>
       </c>
       <c r="C45" s="31">
-        <f t="shared" ref="C45:H45" si="18">C29/C37</f>
+        <f t="shared" ref="C45:H45" si="12">C29/C37</f>
         <v>16776.734693877552</v>
       </c>
       <c r="D45" s="31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>18802.8</v>
       </c>
       <c r="E45" s="31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>11288.5</v>
       </c>
       <c r="F45" s="31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>13331.377358490567</v>
       </c>
       <c r="G45" s="31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="12"/>
         <v>16137.094339622641</v>
       </c>
-      <c r="H45" s="49">
-        <f t="shared" si="18"/>
+      <c r="H45" s="48">
+        <f t="shared" si="12"/>
         <v>19305.64</v>
       </c>
       <c r="J45" s="31">
-        <f t="shared" si="12"/>
+        <f t="shared" si="8"/>
+        <v>-639.64035425491056</v>
+      </c>
+      <c r="K45" s="44">
+        <f t="shared" si="9"/>
+        <v>-3.8126629879194462E-2</v>
+      </c>
+      <c r="M45" s="31">
+        <f>H45-D45</f>
         <v>502.84000000000015</v>
       </c>
-      <c r="K45" s="45">
-        <f t="shared" si="13"/>
+      <c r="N45" s="44">
+        <f>H45/D45-1</f>
         <v>2.6742825536622217E-2</v>
       </c>
-      <c r="M45" s="31">
-        <f t="shared" si="14"/>
+      <c r="P45" s="31">
+        <f>SUM(G45:H45)-SUM(C45:D45)</f>
         <v>-136.80035425490496</v>
       </c>
-      <c r="N45" s="45">
-        <f t="shared" si="15"/>
+      <c r="Q45" s="44">
+        <f>SUM(G45:H45)/SUM(C45:D45)-1</f>
         <v>-3.8449169004575179E-3</v>
       </c>
     </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B47" s="18" t="s">
+        <v>960</v>
+      </c>
+      <c r="M47" s="50"/>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B48" s="18" t="s">
+        <v>961</v>
+      </c>
+    </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B49" s="3" t="s">
-        <v>947</v>
+      <c r="B49" s="51" t="s">
+        <v>962</v>
       </c>
     </row>
     <row r="50" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B50" s="3" t="s">
-        <v>948</v>
+      <c r="B50" s="51" t="s">
+        <v>963</v>
       </c>
     </row>
     <row r="51" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B51" s="3" t="s">
-        <v>949</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B52" s="3" t="s">
-        <v>950</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B55" s="23" t="s">
-        <v>953</v>
-      </c>
+      <c r="B51" s="51"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" s="23"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" s="23"/>
     </row>
     <row r="56" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B56" s="23" t="s">
-        <v>954</v>
-      </c>
+      <c r="B56" s="23"/>
     </row>
     <row r="58" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B58" s="23" t="s">
-        <v>955</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B60" s="23" t="s">
-        <v>956</v>
-      </c>
+      <c r="B58" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30541,7 +30812,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="8" id="{CEE82153-BA13-47BE-9239-ACC0A04E6262}">
+          <x14:cfRule type="iconSet" priority="13" id="{CEE82153-BA13-47BE-9239-ACC0A04E6262}">
             <x14:iconSet iconSet="3Triangles">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -30557,7 +30828,119 @@
           <xm:sqref>C7</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="7" id="{E512727B-3884-4032-BCB0-D25858D03DC6}">
+          <x14:cfRule type="iconSet" priority="12" id="{E512727B-3884-4032-BCB0-D25858D03DC6}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>N25:N29</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="11" id="{1FD74CE5-4633-4699-8E34-6E38153DA2FA}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>Q25:Q29</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="10" id="{9E9F1AFB-4FF5-48FF-9A91-D8A980E62C7F}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>N33:N37</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="9" id="{FF421590-3484-46D9-AF4D-EA6620EC0191}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>Q33:Q37</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="8" id="{A980C32E-5FD8-404D-A7C8-7E3F5E1B2421}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>G7</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="7" id="{6C4D67D8-9DCA-4746-BC9F-C0B3A9107BF7}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>N41:N45</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="6" id="{E192AF3B-D71C-4D46-9813-A6B7A5A2F07F}">
+            <x14:iconSet iconSet="3Triangles">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num" gte="0">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>Q41:Q45</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="5" id="{8C6D02BB-B37A-4CC9-9049-30E3DDA90BED}">
             <x14:iconSet iconSet="3Triangles">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -30573,23 +30956,7 @@
           <xm:sqref>K25:K29</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="6" id="{1FD74CE5-4633-4699-8E34-6E38153DA2FA}">
-            <x14:iconSet iconSet="3Triangles">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>N25:N29</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="5" id="{9E9F1AFB-4FF5-48FF-9A91-D8A980E62C7F}">
+          <x14:cfRule type="iconSet" priority="2" id="{8FA7640A-7FE8-45CA-8C2E-B2A03B1F53F1}">
             <x14:iconSet iconSet="3Triangles">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -30605,39 +30972,7 @@
           <xm:sqref>K33:K37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="4" id="{FF421590-3484-46D9-AF4D-EA6620EC0191}">
-            <x14:iconSet iconSet="3Triangles">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>N33:N37</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="3" id="{A980C32E-5FD8-404D-A7C8-7E3F5E1B2421}">
-            <x14:iconSet iconSet="3Triangles">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>F7</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="2" id="{6C4D67D8-9DCA-4746-BC9F-C0B3A9107BF7}">
+          <x14:cfRule type="iconSet" priority="1" id="{FD50ADC7-F05F-4AE8-9E42-303134169A3F}">
             <x14:iconSet iconSet="3Triangles">
               <x14:cfvo type="percent">
                 <xm:f>0</xm:f>
@@ -30651,22 +30986,6 @@
             </x14:iconSet>
           </x14:cfRule>
           <xm:sqref>K41:K45</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="iconSet" priority="1" id="{E192AF3B-D71C-4D46-9813-A6B7A5A2F07F}">
-            <x14:iconSet iconSet="3Triangles">
-              <x14:cfvo type="percent">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num" gte="0">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-            </x14:iconSet>
-          </x14:cfRule>
-          <xm:sqref>N41:N45</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>